<commit_message>
add all work at once
</commit_message>
<xml_diff>
--- a/uji_data_hujan_obs/PCH_bilibili/lon_lat_PCH.xlsx
+++ b/uji_data_hujan_obs/PCH_bilibili/lon_lat_PCH.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rahma\SW Bilibili\RAAT\Hasil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Happy\satellite_correction\uji_data_hujan_obs\PCH_bilibili\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41557117-DC83-4B92-8464-EDEAF98A4439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EF4919-20E9-48C5-BD2A-D7DE9CDE1169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10935" yWindow="1155" windowWidth="26160" windowHeight="14400" xr2:uid="{9F7FD5C0-D8AD-4792-8CD1-D1D7819FE593}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F7FD5C0-D8AD-4792-8CD1-D1D7819FE593}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="23">
   <si>
     <t>PCH STASIUN BILI-BILI</t>
   </si>
@@ -67,17 +68,45 @@
   </si>
   <si>
     <t>Latitude</t>
+  </si>
+  <si>
+    <t>pch asal</t>
+  </si>
+  <si>
+    <t>pch acuan</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>PCH STASIUN KD2</t>
+  </si>
+  <si>
+    <t>PCH STASIUN KD3</t>
+  </si>
+  <si>
+    <t>PCH STASIUN KD4</t>
+  </si>
+  <si>
+    <t>PCH STASIUN KD5</t>
+  </si>
+  <si>
+    <t>PCH STASIUN KD6</t>
+  </si>
+  <si>
+    <t>PCH STASIUN KD7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +119,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,15 +165,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,31 +490,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3DB1A8-1808-4627-A38F-588D374962E0}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F2" sqref="F2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>-5.2491000000000003</v>
+      </c>
+      <c r="D2" s="4">
+        <v>119.5788</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>-5.2869440000000001</v>
+      </c>
+      <c r="D3" s="5">
+        <v>119.517222</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-5.2738889999999996</v>
+      </c>
+      <c r="D4" s="5">
+        <v>119.743611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5">
+        <v>-5.3022220000000004</v>
+      </c>
+      <c r="D5" s="5">
+        <v>119.88722199999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>-5.3627779999999996</v>
+      </c>
+      <c r="D6" s="5">
+        <v>119.734722</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>-5.1924999999999999</v>
+      </c>
+      <c r="D7" s="5">
+        <v>119.418333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-5.2527780000000002</v>
+      </c>
+      <c r="D8" s="5">
+        <v>119.85333300000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5">
+        <v>-5.3352779999999997</v>
+      </c>
+      <c r="D9" s="5">
+        <v>119.680556</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>-5.2905559999999996</v>
+      </c>
+      <c r="D10" s="5">
+        <v>119.87305600000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-5.2991669999999997</v>
+      </c>
+      <c r="D11" s="5">
+        <v>119.90222199999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C8C86C-54E4-4ABC-B464-89D3927914C2}">
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>12</v>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -487,138 +704,538 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4">
-        <v>-5.2491000000000003</v>
-      </c>
-      <c r="D2" s="4">
-        <v>119.5788</v>
-      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
-        <v>-5.2869440000000001</v>
-      </c>
-      <c r="D3" s="5">
-        <v>119.517222</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5">
-        <v>-5.2738889999999996</v>
-      </c>
-      <c r="D4" s="5">
-        <v>119.743611</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5">
-        <v>-5.3022220000000004</v>
-      </c>
-      <c r="D5" s="5">
-        <v>119.88722199999999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
-        <v>-5.3627779999999996</v>
-      </c>
-      <c r="D6" s="5">
-        <v>119.734722</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5">
-        <v>-5.1924999999999999</v>
-      </c>
-      <c r="D7" s="5">
-        <v>119.418333</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5">
-        <v>-5.2527780000000002</v>
-      </c>
-      <c r="D8" s="5">
-        <v>119.85333300000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5">
-        <v>-5.3352779999999997</v>
-      </c>
-      <c r="D9" s="5">
-        <v>119.680556</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5">
-        <v>-5.2905559999999996</v>
-      </c>
-      <c r="D10" s="5">
-        <v>119.87305600000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5">
-        <v>-5.2991669999999997</v>
-      </c>
-      <c r="D11" s="5">
-        <v>119.90222199999999</v>
-      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>